<commit_message>
initial phase of project
</commit_message>
<xml_diff>
--- a/static/media/aero@gmail.com/resources/products.xlsx
+++ b/static/media/aero@gmail.com/resources/products.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -463,330 +463,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>proudct1</t>
+          <t>Product 2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SKJKLffjskljlkfs</t>
+          <t>product A category</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>kdjlkjkldJLKJLKdgjlk</t>
+          <t>It is a long established fact that a reader will be distracted by the readable content of a page when looking at its layout. The point of using Lorem Ipsum is that it has a more-or-less normal distribution of letters, as opposed to using 'Content here, content here', making it look like readable English.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>JFJFJKJKFJKLFJKLSJLKF</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>JFSJKJKFJFJajfkljkl</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>dfkjklfjlkdglkjljk</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>kfjdjkldjklJKLdgjlg</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>jkfjkjkfJLFJLKJLDJKLd</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>dJKLKGkldjlgjldk</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>kdkkldgkgdkl</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>kldklfdjkldgkljkljGD</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>KJLFDJKLDLJKGljkdgjlkg</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>JFSJKJKFJFJajfkljkl</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>dfkjklfjlkdglkjljk</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>kfjdjkldjklJKLdgjlg</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>jkfjkjkfJLFJLKJLDJKLd</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>dJKLKGkldjlgjldk</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>kdkkldgkgdkl</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>kldklfdjkldgkljkljGD</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>KJLFDJKLDLJKGljkdgjlkg</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>proudct1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>SKJKLffjskljlkfs</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>kdjlkjkldJLKJLKdgjlk</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>JFJFJKJKFJKLFJKLSJLKF</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>JFSJKJKFJFJajfkljkl</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>dfkjklfjlkdglkjljk</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>kfjdjkldjklJKLdgjlg</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>jkfjkjkfJLFJLKJLDJKLd</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>dJKLKGkldjlgjldk</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>kdkkldgkgdkl</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>kldklfdjkldgkljkljGD</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>KJLFDJKLDLJKGljkdgjlkg</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>JFSJKJKFJFJajfkljkl</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>dfkjklfjlkdglkjljk</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>kfjdjkldjklJKLdgjlg</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>jkfjkjkfJLFJLKJLDJKLd</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>dJKLKGkldjlgjldk</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>kdkkldgkgdkl</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>kldklfdjkldgkljkljGD</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>KJLFDJKLDLJKGljkdgjlkg</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>proudct1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>SKJKLffjskljlkfs</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>kdjlkjkldJLKJLKdgjlk</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>JFJFJKJKFJKLFJKLSJLKF</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>JFSJKJKFJFJajfkljkl</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>dfkjklfjlkdglkjljk</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>kfjdjkldjklJKLdgjlg</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>jkfjkjkfJLFJLKJLDJKLd</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>dJKLKGkldjlgjldk</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>kdkkldgkgdkl</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>kldklfdjkldgkljkljGD</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>KJLFDJKLDLJKGljkdgjlkg</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>JFSJKJKFJFJajfkljkl</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>dfkjklfjlkdglkjljk</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>kfjdjkldjklJKLdgjlg</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>jkfjkjkfJLFJLKJLDJKLd</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>dJKLKGkldjlgjldk</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>kdkkldgkgdkl</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>kldklfdjkldgkljkljGD</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>KJLFDJKLDLJKGljkdgjlkg</t>
+          <t>http://www.google.com</t>
         </is>
       </c>
     </row>

</xml_diff>